<commit_message>
(1) Updated Random Effects Structure in the Meta-Analysis, (2) Modifications to the Testing of Various Random Effects Structures, (3) Addition of an Evidence and Gap Map
</commit_message>
<xml_diff>
--- a/DATA/OUTPUT_FROM_R/SAVED_OBJECTS_FROM_R/relative_aic_bic_adjusted.xlsx
+++ b/DATA/OUTPUT_FROM_R/SAVED_OBJECTS_FROM_R/relative_aic_bic_adjusted.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">Interaction Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Greenhouse gas emission</t>
+    <t xml:space="preserve">Carbon sequestration</t>
   </si>
   <si>
     <t xml:space="preserve">Product quality</t>
@@ -440,10 +440,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>880452.15085856</v>
+        <v>931028.30798162</v>
       </c>
       <c r="D2" t="n">
-        <v>880455.360344713</v>
+        <v>931031.517467773</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -452,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-440225.07542928</v>
+        <v>-465513.15399081</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -469,25 +469,25 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>878010.420848356</v>
+        <v>895505.014562306</v>
       </c>
       <c r="D3" t="n">
-        <v>878020.049306814</v>
+        <v>895517.852506917</v>
       </c>
       <c r="E3" t="n">
-        <v>-2441.73001020402</v>
+        <v>-35523.2934193138</v>
       </c>
       <c r="F3" t="n">
-        <v>-2435.3110378983</v>
+        <v>-35513.6649608554</v>
       </c>
       <c r="G3" t="n">
-        <v>-439002.210424178</v>
+        <v>-447748.507281153</v>
       </c>
       <c r="H3" t="n">
-        <v>2441.73001020402</v>
+        <v>35523.2934193138</v>
       </c>
       <c r="I3" t="n">
-        <v>2435.3110378983</v>
+        <v>35513.6649608554</v>
       </c>
     </row>
     <row r="4">
@@ -498,25 +498,25 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>877410.202578311</v>
+        <v>895284.911670573</v>
       </c>
       <c r="D4" t="n">
-        <v>877423.519624542</v>
+        <v>895300.448224509</v>
       </c>
       <c r="E4" t="n">
-        <v>-3041.94828024902</v>
+        <v>-35743.396311047</v>
       </c>
       <c r="F4" t="n">
-        <v>-3031.84072017088</v>
+        <v>-35731.0692432637</v>
       </c>
       <c r="G4" t="n">
-        <v>-438699.101289155</v>
+        <v>-447635.455835286</v>
       </c>
       <c r="H4" t="n">
-        <v>3041.94828024902</v>
+        <v>35743.396311047</v>
       </c>
       <c r="I4" t="n">
-        <v>3031.84072017088</v>
+        <v>35731.0692432637</v>
       </c>
     </row>
     <row r="5">
@@ -527,25 +527,25 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>877410.202578311</v>
+        <v>895284.911670573</v>
       </c>
       <c r="D5" t="n">
-        <v>877423.519624542</v>
+        <v>895300.448224509</v>
       </c>
       <c r="E5" t="n">
-        <v>-3041.94828024902</v>
+        <v>-35743.396311047</v>
       </c>
       <c r="F5" t="n">
-        <v>-3031.84072017088</v>
+        <v>-35731.0692432637</v>
       </c>
       <c r="G5" t="n">
-        <v>-438699.101289155</v>
+        <v>-447635.455835286</v>
       </c>
       <c r="H5" t="n">
-        <v>3041.94828024902</v>
+        <v>35743.396311047</v>
       </c>
       <c r="I5" t="n">
-        <v>3031.84072017088</v>
+        <v>35731.0692432637</v>
       </c>
     </row>
     <row r="6">
@@ -556,10 +556,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>5437.01058252294</v>
+        <v>3070.87245000935</v>
       </c>
       <c r="D6" t="n">
-        <v>5439.57493071441</v>
+        <v>3073.43679820082</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-2717.50529126147</v>
+        <v>-1534.43622500468</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -585,25 +585,25 @@
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>5441.01058252331</v>
+        <v>3076.87245000935</v>
       </c>
       <c r="D7" t="n">
-        <v>5448.70362709772</v>
+        <v>3087.12984277522</v>
       </c>
       <c r="E7" t="n">
-        <v>4.00000000037471</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>9.12869638331085</v>
+        <v>13.6930445744038</v>
       </c>
       <c r="G7" t="n">
-        <v>-2717.50529126166</v>
+        <v>-1534.43622500468</v>
       </c>
       <c r="H7" t="n">
-        <v>4.00000000037471</v>
+        <v>6</v>
       </c>
       <c r="I7" t="n">
-        <v>9.12869638331085</v>
+        <v>13.6930445744038</v>
       </c>
     </row>
     <row r="8">
@@ -614,25 +614,25 @@
         <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>2284.2824841589</v>
+        <v>1545.19897941258</v>
       </c>
       <c r="D8" t="n">
-        <v>2294.32592218497</v>
+        <v>1555.24241743864</v>
       </c>
       <c r="E8" t="n">
-        <v>-3152.72809836404</v>
+        <v>-1525.67347059677</v>
       </c>
       <c r="F8" t="n">
-        <v>-3145.24900852944</v>
+        <v>-1518.19438076217</v>
       </c>
       <c r="G8" t="n">
-        <v>-1138.14124207945</v>
+        <v>-768.599489706289</v>
       </c>
       <c r="H8" t="n">
-        <v>3152.72809836404</v>
+        <v>1525.67347059677</v>
       </c>
       <c r="I8" t="n">
-        <v>3145.24900852944</v>
+        <v>1518.19438076217</v>
       </c>
     </row>
     <row r="9">
@@ -643,25 +643,25 @@
         <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>2289.55172877215</v>
+        <v>1556.29495988232</v>
       </c>
       <c r="D9" t="n">
-        <v>2302.0507771238</v>
+        <v>1568.79400823398</v>
       </c>
       <c r="E9" t="n">
-        <v>-3147.45885375079</v>
+        <v>-1514.57749012703</v>
       </c>
       <c r="F9" t="n">
-        <v>-3137.52415359061</v>
+        <v>-1504.64278996684</v>
       </c>
       <c r="G9" t="n">
-        <v>-1139.77586438607</v>
+        <v>-773.147479941162</v>
       </c>
       <c r="H9" t="n">
-        <v>3147.45885375079</v>
+        <v>1514.57749012703</v>
       </c>
       <c r="I9" t="n">
-        <v>3137.52415359061</v>
+        <v>1504.64278996684</v>
       </c>
     </row>
     <row r="10">
@@ -672,10 +672,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>-300.786571977615</v>
+        <v>-499.538321721254</v>
       </c>
       <c r="D10" t="n">
-        <v>-298.123132883503</v>
+        <v>-496.874882627142</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>151.393285988808</v>
+        <v>250.769160860627</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -701,25 +701,25 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>-309.905624538861</v>
+        <v>-508.522975782897</v>
       </c>
       <c r="D11" t="n">
-        <v>-301.915307256525</v>
+        <v>-497.869219406449</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.11905256124533</v>
+        <v>-8.98465406164291</v>
       </c>
       <c r="F11" t="n">
-        <v>-3.79217437302117</v>
+        <v>-0.994336779306707</v>
       </c>
       <c r="G11" t="n">
-        <v>157.95281226943</v>
+        <v>258.261487891448</v>
       </c>
       <c r="H11" t="n">
-        <v>9.11905256124533</v>
+        <v>8.98465406164291</v>
       </c>
       <c r="I11" t="n">
-        <v>3.79217437302117</v>
+        <v>0.994336779306707</v>
       </c>
     </row>
     <row r="12">
@@ -730,25 +730,25 @@
         <v>12</v>
       </c>
       <c r="C12" t="n">
-        <v>-96.8690436586897</v>
+        <v>-163.465739884609</v>
       </c>
       <c r="D12" t="n">
-        <v>-83.6774205334922</v>
+        <v>-148.808380856611</v>
       </c>
       <c r="E12" t="n">
-        <v>203.917528318926</v>
+        <v>336.072581836645</v>
       </c>
       <c r="F12" t="n">
-        <v>214.445712350011</v>
+        <v>348.066501770531</v>
       </c>
       <c r="G12" t="n">
-        <v>57.4345218293449</v>
+        <v>91.7328699423043</v>
       </c>
       <c r="H12" t="n">
-        <v>203.917528318926</v>
+        <v>336.072581836645</v>
       </c>
       <c r="I12" t="n">
-        <v>214.445712350011</v>
+        <v>348.066501770531</v>
       </c>
     </row>
     <row r="13">
@@ -759,25 +759,25 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>-96.8690436586897</v>
+        <v>-163.465739884609</v>
       </c>
       <c r="D13" t="n">
-        <v>-83.6774205334922</v>
+        <v>-148.808380856611</v>
       </c>
       <c r="E13" t="n">
-        <v>203.917528318926</v>
+        <v>336.072581836645</v>
       </c>
       <c r="F13" t="n">
-        <v>214.445712350011</v>
+        <v>348.066501770531</v>
       </c>
       <c r="G13" t="n">
-        <v>57.4345218293449</v>
+        <v>91.7328699423043</v>
       </c>
       <c r="H13" t="n">
-        <v>203.917528318926</v>
+        <v>336.072581836645</v>
       </c>
       <c r="I13" t="n">
-        <v>214.445712350011</v>
+        <v>348.066501770531</v>
       </c>
     </row>
     <row r="14">
@@ -788,10 +788,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>201796.894893716</v>
+        <v>189796.318141784</v>
       </c>
       <c r="D14" t="n">
-        <v>201800.515294582</v>
+        <v>189799.938542649</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>-100897.447446858</v>
+        <v>-94897.1590708918</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -817,25 +817,25 @@
         <v>11</v>
       </c>
       <c r="C15" t="n">
-        <v>92947.5392110831</v>
+        <v>82352.0425680329</v>
       </c>
       <c r="D15" t="n">
-        <v>92958.4004136803</v>
+        <v>82366.5241714958</v>
       </c>
       <c r="E15" t="n">
-        <v>-108849.355682633</v>
+        <v>-107444.275573751</v>
       </c>
       <c r="F15" t="n">
-        <v>-108842.114880902</v>
+        <v>-107433.414371154</v>
       </c>
       <c r="G15" t="n">
-        <v>-46470.7696055416</v>
+        <v>-41172.0212840165</v>
       </c>
       <c r="H15" t="n">
-        <v>108849.355682633</v>
+        <v>107444.275573751</v>
       </c>
       <c r="I15" t="n">
-        <v>108842.114880902</v>
+        <v>107433.414371154</v>
       </c>
     </row>
     <row r="16">
@@ -846,25 +846,25 @@
         <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>7182.97726283379</v>
+        <v>6337.35754896603</v>
       </c>
       <c r="D16" t="n">
-        <v>7227.93544694025</v>
+        <v>6385.31294534625</v>
       </c>
       <c r="E16" t="n">
-        <v>-194613.917630883</v>
+        <v>-183458.960592818</v>
       </c>
       <c r="F16" t="n">
-        <v>-194572.579847642</v>
+        <v>-183414.625597303</v>
       </c>
       <c r="G16" t="n">
-        <v>-3576.48863141689</v>
+        <v>-3152.67877448301</v>
       </c>
       <c r="H16" t="n">
-        <v>194613.917630883</v>
+        <v>183458.960592818</v>
       </c>
       <c r="I16" t="n">
-        <v>194572.579847642</v>
+        <v>183414.625597303</v>
       </c>
     </row>
     <row r="17">
@@ -875,25 +875,25 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>6806.02968348186</v>
+        <v>6157.4927272959</v>
       </c>
       <c r="D17" t="n">
-        <v>6892.74015732852</v>
+        <v>6247.09355027078</v>
       </c>
       <c r="E17" t="n">
-        <v>-194990.865210235</v>
+        <v>-183638.825414488</v>
       </c>
       <c r="F17" t="n">
-        <v>-194907.775137254</v>
+        <v>-183552.844992379</v>
       </c>
       <c r="G17" t="n">
-        <v>-3373.01484174093</v>
+        <v>-3047.74636364795</v>
       </c>
       <c r="H17" t="n">
-        <v>194990.865210235</v>
+        <v>183638.825414488</v>
       </c>
       <c r="I17" t="n">
-        <v>194907.775137254</v>
+        <v>183552.844992379</v>
       </c>
     </row>
     <row r="18">
@@ -904,10 +904,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>86614.9401791614</v>
+        <v>119396.850936627</v>
       </c>
       <c r="D18" t="n">
-        <v>86616.8113801723</v>
+        <v>119398.722137638</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>-43306.4700895807</v>
+        <v>-59697.4254683136</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -933,25 +933,25 @@
         <v>11</v>
       </c>
       <c r="C19" t="n">
-        <v>81455.174132281</v>
+        <v>115863.294437099</v>
       </c>
       <c r="D19" t="n">
-        <v>81460.7877353138</v>
+        <v>115870.779241143</v>
       </c>
       <c r="E19" t="n">
-        <v>-5159.76604688035</v>
+        <v>-3533.55649952796</v>
       </c>
       <c r="F19" t="n">
-        <v>-5156.02364485853</v>
+        <v>-3527.94289649522</v>
       </c>
       <c r="G19" t="n">
-        <v>-40724.5870661405</v>
+        <v>-57927.6472185496</v>
       </c>
       <c r="H19" t="n">
-        <v>5159.76604688035</v>
+        <v>3533.55649952796</v>
       </c>
       <c r="I19" t="n">
-        <v>5156.02364485853</v>
+        <v>3527.94289649522</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
         <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>76727.772246882</v>
+        <v>109150.955636152</v>
       </c>
       <c r="D20" t="n">
-        <v>76727.1585412432</v>
+        <v>109150.341930513</v>
       </c>
       <c r="E20" t="n">
-        <v>-9887.16793227935</v>
+        <v>-10245.8953004748</v>
       </c>
       <c r="F20" t="n">
-        <v>-9889.65283892913</v>
+        <v>-10248.3802071246</v>
       </c>
       <c r="G20" t="n">
-        <v>-38362.886123441</v>
+        <v>-54574.4778180761</v>
       </c>
       <c r="H20" t="n">
-        <v>9887.16793227935</v>
+        <v>10245.8953004748</v>
       </c>
       <c r="I20" t="n">
-        <v>9889.65283892913</v>
+        <v>10248.3802071246</v>
       </c>
     </row>
     <row r="21">
@@ -991,25 +991,25 @@
         <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>76727.772246882</v>
+        <v>109150.955636152</v>
       </c>
       <c r="D21" t="n">
-        <v>76727.1585412432</v>
+        <v>109150.341930513</v>
       </c>
       <c r="E21" t="n">
-        <v>-9887.16793227935</v>
+        <v>-10245.8953004748</v>
       </c>
       <c r="F21" t="n">
-        <v>-9889.65283892913</v>
+        <v>-10248.3802071246</v>
       </c>
       <c r="G21" t="n">
-        <v>-38362.886123441</v>
+        <v>-54574.4778180761</v>
       </c>
       <c r="H21" t="n">
-        <v>9887.16793227935</v>
+        <v>10245.8953004748</v>
       </c>
       <c r="I21" t="n">
-        <v>9889.65283892913</v>
+        <v>10248.3802071246</v>
       </c>
     </row>
     <row r="22">
@@ -1020,10 +1020,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>1924997.93297406</v>
+        <v>9817492.65391331</v>
       </c>
       <c r="D22" t="n">
-        <v>1925001.45443498</v>
+        <v>9817496.17537423</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>-962497.966487032</v>
+        <v>-4908745.32695665</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1049,25 +1049,25 @@
         <v>11</v>
       </c>
       <c r="C23" t="n">
-        <v>137778.335596123</v>
+        <v>242380.234257061</v>
       </c>
       <c r="D23" t="n">
-        <v>137788.899978876</v>
+        <v>242394.320100732</v>
       </c>
       <c r="E23" t="n">
-        <v>-1787219.59737794</v>
+        <v>-9575112.41965625</v>
       </c>
       <c r="F23" t="n">
-        <v>-1787212.55445611</v>
+        <v>-9575101.85527349</v>
       </c>
       <c r="G23" t="n">
-        <v>-68886.1677980613</v>
+        <v>-121186.11712853</v>
       </c>
       <c r="H23" t="n">
-        <v>1787219.59737794</v>
+        <v>9575112.41965625</v>
       </c>
       <c r="I23" t="n">
-        <v>1787212.55445611</v>
+        <v>9575101.85527349</v>
       </c>
     </row>
     <row r="24">
@@ -1078,25 +1078,25 @@
         <v>12</v>
       </c>
       <c r="C24" t="n">
-        <v>135720.987788942</v>
+        <v>235109.006440944</v>
       </c>
       <c r="D24" t="n">
-        <v>135735.289147816</v>
+        <v>235125.350851087</v>
       </c>
       <c r="E24" t="n">
-        <v>-1789276.94518512</v>
+        <v>-9582383.64747236</v>
       </c>
       <c r="F24" t="n">
-        <v>-1789266.16528717</v>
+        <v>-9582370.82452314</v>
       </c>
       <c r="G24" t="n">
-        <v>-67853.4938944708</v>
+        <v>-117546.503220472</v>
       </c>
       <c r="H24" t="n">
-        <v>1789276.94518512</v>
+        <v>9582383.64747236</v>
       </c>
       <c r="I24" t="n">
-        <v>1789266.16528717</v>
+        <v>9582370.82452314</v>
       </c>
     </row>
     <row r="25">
@@ -1107,25 +1107,25 @@
         <v>13</v>
       </c>
       <c r="C25" t="n">
-        <v>135720.987788942</v>
+        <v>235109.006440944</v>
       </c>
       <c r="D25" t="n">
-        <v>135735.289147816</v>
+        <v>235125.350851087</v>
       </c>
       <c r="E25" t="n">
-        <v>-1789276.94518512</v>
+        <v>-9582383.64747236</v>
       </c>
       <c r="F25" t="n">
-        <v>-1789266.16528717</v>
+        <v>-9582370.82452314</v>
       </c>
       <c r="G25" t="n">
-        <v>-67853.4938944708</v>
+        <v>-117546.503220472</v>
       </c>
       <c r="H25" t="n">
-        <v>1789276.94518512</v>
+        <v>9582383.64747236</v>
       </c>
       <c r="I25" t="n">
-        <v>1789266.16528717</v>
+        <v>9582370.82452314</v>
       </c>
     </row>
     <row r="26">
@@ -1136,10 +1136,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="n">
-        <v>1408.15679456153</v>
+        <v>1328.1060261503</v>
       </c>
       <c r="D26" t="n">
-        <v>1411.01660696589</v>
+        <v>1330.96583855466</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>-703.078397280763</v>
+        <v>-663.05301307515</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -1165,25 +1165,25 @@
         <v>11</v>
       </c>
       <c r="C27" t="n">
-        <v>1200.0087608442</v>
+        <v>1131.26013147114</v>
       </c>
       <c r="D27" t="n">
-        <v>1205.72838565292</v>
+        <v>1136.97975627986</v>
       </c>
       <c r="E27" t="n">
-        <v>-208.148033717327</v>
+        <v>-196.84589467916</v>
       </c>
       <c r="F27" t="n">
-        <v>-205.288221312966</v>
+        <v>-193.986082274798</v>
       </c>
       <c r="G27" t="n">
-        <v>-598.004380422099</v>
+        <v>-563.63006573557</v>
       </c>
       <c r="H27" t="n">
-        <v>208.148033717327</v>
+        <v>196.84589467916</v>
       </c>
       <c r="I27" t="n">
-        <v>205.288221312966</v>
+        <v>193.986082274798</v>
       </c>
     </row>
     <row r="28">
@@ -1194,25 +1194,25 @@
         <v>12</v>
       </c>
       <c r="C28" t="n">
-        <v>1215.92779080522</v>
+        <v>1154.91358263294</v>
       </c>
       <c r="D28" t="n">
-        <v>1227.30453915106</v>
+        <v>1166.29033097877</v>
       </c>
       <c r="E28" t="n">
-        <v>-192.229003756301</v>
+        <v>-173.192443517362</v>
       </c>
       <c r="F28" t="n">
-        <v>-183.712067814828</v>
+        <v>-164.675507575889</v>
       </c>
       <c r="G28" t="n">
-        <v>-603.963895402612</v>
+        <v>-573.456791316469</v>
       </c>
       <c r="H28" t="n">
-        <v>192.229003756301</v>
+        <v>173.192443517362</v>
       </c>
       <c r="I28" t="n">
-        <v>183.712067814828</v>
+        <v>164.675507575889</v>
       </c>
     </row>
     <row r="29">
@@ -1223,25 +1223,25 @@
         <v>13</v>
       </c>
       <c r="C29" t="n">
-        <v>1215.92779080522</v>
+        <v>1154.91358263294</v>
       </c>
       <c r="D29" t="n">
-        <v>1227.30453915106</v>
+        <v>1166.29033097877</v>
       </c>
       <c r="E29" t="n">
-        <v>-192.229003756301</v>
+        <v>-173.192443517362</v>
       </c>
       <c r="F29" t="n">
-        <v>-183.712067814828</v>
+        <v>-164.675507575889</v>
       </c>
       <c r="G29" t="n">
-        <v>-603.963895402612</v>
+        <v>-573.456791316469</v>
       </c>
       <c r="H29" t="n">
-        <v>192.229003756301</v>
+        <v>173.192443517362</v>
       </c>
       <c r="I29" t="n">
-        <v>183.712067814828</v>
+        <v>164.675507575889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After meeting with Maarit: (1) Removing intercept is fine, (2) Adjusting random effects structure, (3) developing 'cabbage-approach' multi-level random effects models with singe moderator models and two-way moderator interaction models, (4) model extraction and evaluation, (5) ANOVA contrast matrix — pairwise comparisons between moderator levels - to be continued!
</commit_message>
<xml_diff>
--- a/DATA/OUTPUT_FROM_R/SAVED_OBJECTS_FROM_R/relative_aic_bic_adjusted.xlsx
+++ b/DATA/OUTPUT_FROM_R/SAVED_OBJECTS_FROM_R/relative_aic_bic_adjusted.xlsx
@@ -50,28 +50,28 @@
     <t xml:space="preserve">Minimal Random Effects Model</t>
   </si>
   <si>
+    <t xml:space="preserve">Carbon sequestration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crop yield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pest and disease control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water quality</t>
+  </si>
+  <si>
     <t xml:space="preserve">Full Model</t>
   </si>
   <si>
     <t xml:space="preserve">Interaction Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbon sequestration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crop yield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pest and Disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water quality</t>
   </si>
 </sst>
 </file>
@@ -440,10 +440,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>931028.30798162</v>
+        <v>912841.032618104</v>
       </c>
       <c r="D2" t="n">
-        <v>931031.517467773</v>
+        <v>912844.242104257</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -452,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-465513.15399081</v>
+        <v>-456419.516309052</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -469,97 +469,97 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>895505.014562306</v>
+        <v>857763.055138436</v>
       </c>
       <c r="D3" t="n">
-        <v>895517.852506917</v>
+        <v>857775.893083047</v>
       </c>
       <c r="E3" t="n">
-        <v>-35523.2934193138</v>
+        <v>-55077.9774796683</v>
       </c>
       <c r="F3" t="n">
-        <v>-35513.6649608554</v>
+        <v>-55068.3490212099</v>
       </c>
       <c r="G3" t="n">
-        <v>-447748.507281153</v>
+        <v>-428877.527569218</v>
       </c>
       <c r="H3" t="n">
-        <v>35523.2934193138</v>
+        <v>55077.9774796683</v>
       </c>
       <c r="I3" t="n">
-        <v>35513.6649608554</v>
+        <v>55068.3490212099</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>895284.911670573</v>
+        <v>3314.50981077785</v>
       </c>
       <c r="D4" t="n">
-        <v>895300.448224509</v>
+        <v>3317.07415896932</v>
       </c>
       <c r="E4" t="n">
-        <v>-35743.396311047</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-35731.0692432637</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-447635.455835286</v>
+        <v>-1656.25490538893</v>
       </c>
       <c r="H4" t="n">
-        <v>35743.396311047</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>35731.0692432637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>895284.911670573</v>
+        <v>3320.50981077785</v>
       </c>
       <c r="D5" t="n">
-        <v>895300.448224509</v>
+        <v>3330.76720354373</v>
       </c>
       <c r="E5" t="n">
-        <v>-35743.396311047</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>-35731.0692432637</v>
+        <v>13.6930445744038</v>
       </c>
       <c r="G5" t="n">
-        <v>-447635.455835286</v>
+        <v>-1656.25490538893</v>
       </c>
       <c r="H5" t="n">
-        <v>35743.396311047</v>
+        <v>6</v>
       </c>
       <c r="I5" t="n">
-        <v>35731.0692432637</v>
+        <v>13.6930445744038</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>3070.87245000935</v>
+        <v>-1052.42668628724</v>
       </c>
       <c r="D6" t="n">
-        <v>3073.43679820082</v>
+        <v>-1049.76324719313</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-1534.43622500468</v>
+        <v>527.213343143619</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -579,31 +579,31 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>3076.87245000935</v>
+        <v>-1046.42668628724</v>
       </c>
       <c r="D7" t="n">
-        <v>3087.12984277522</v>
+        <v>-1035.77292991079</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>13.6930445744038</v>
+        <v>13.990317282336</v>
       </c>
       <c r="G7" t="n">
-        <v>-1534.43622500468</v>
+        <v>527.213343143619</v>
       </c>
       <c r="H7" t="n">
         <v>6</v>
       </c>
       <c r="I7" t="n">
-        <v>13.6930445744038</v>
+        <v>13.990317282336</v>
       </c>
     </row>
     <row r="8">
@@ -611,28 +611,28 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>1545.19897941258</v>
+        <v>184934.185069212</v>
       </c>
       <c r="D8" t="n">
-        <v>1555.24241743864</v>
+        <v>184937.805470078</v>
       </c>
       <c r="E8" t="n">
-        <v>-1525.67347059677</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-1518.19438076217</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-768.599489706289</v>
+        <v>-92466.0925346062</v>
       </c>
       <c r="H8" t="n">
-        <v>1525.67347059677</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1518.19438076217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -640,28 +640,28 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>1556.29495988232</v>
+        <v>78012.7803566418</v>
       </c>
       <c r="D9" t="n">
-        <v>1568.79400823398</v>
+        <v>78027.2619601046</v>
       </c>
       <c r="E9" t="n">
-        <v>-1514.57749012703</v>
+        <v>-106921.404712571</v>
       </c>
       <c r="F9" t="n">
-        <v>-1504.64278996684</v>
+        <v>-106910.543509973</v>
       </c>
       <c r="G9" t="n">
-        <v>-773.147479941162</v>
+        <v>-39002.3901783209</v>
       </c>
       <c r="H9" t="n">
-        <v>1514.57749012703</v>
+        <v>106921.404712571</v>
       </c>
       <c r="I9" t="n">
-        <v>1504.64278996684</v>
+        <v>106910.543509973</v>
       </c>
     </row>
     <row r="10">
@@ -672,10 +672,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>-499.538321721254</v>
+        <v>107687.394895377</v>
       </c>
       <c r="D10" t="n">
-        <v>-496.874882627142</v>
+        <v>107689.266096388</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>250.769160860627</v>
+        <v>-53842.6974476885</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -701,97 +701,97 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>-508.522975782897</v>
+        <v>98496.401157418</v>
       </c>
       <c r="D11" t="n">
-        <v>-497.869219406449</v>
+        <v>98503.8859614616</v>
       </c>
       <c r="E11" t="n">
-        <v>-8.98465406164291</v>
+        <v>-9190.99373795901</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.994336779306707</v>
+        <v>-9185.38013492628</v>
       </c>
       <c r="G11" t="n">
-        <v>258.261487891448</v>
+        <v>-49244.200578709</v>
       </c>
       <c r="H11" t="n">
-        <v>8.98465406164291</v>
+        <v>9190.99373795901</v>
       </c>
       <c r="I11" t="n">
-        <v>0.994336779306707</v>
+        <v>9185.38013492628</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>-163.465739884609</v>
+        <v>872334001.695813</v>
       </c>
       <c r="D12" t="n">
-        <v>-148.808380856611</v>
+        <v>872334005.217274</v>
       </c>
       <c r="E12" t="n">
-        <v>336.072581836645</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>348.066501770531</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>91.7328699423043</v>
+        <v>-436166999.847907</v>
       </c>
       <c r="H12" t="n">
-        <v>336.072581836645</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>348.066501770531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>-163.465739884609</v>
+        <v>14548834.4081621</v>
       </c>
       <c r="D13" t="n">
-        <v>-148.808380856611</v>
+        <v>14548848.4940058</v>
       </c>
       <c r="E13" t="n">
-        <v>336.072581836645</v>
+        <v>-857785167.287651</v>
       </c>
       <c r="F13" t="n">
-        <v>348.066501770531</v>
+        <v>-857785156.723268</v>
       </c>
       <c r="G13" t="n">
-        <v>91.7328699423043</v>
+        <v>-7274413.20408105</v>
       </c>
       <c r="H13" t="n">
-        <v>336.072581836645</v>
+        <v>857785167.287651</v>
       </c>
       <c r="I13" t="n">
-        <v>348.066501770531</v>
+        <v>857785156.723268</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>189796.318141784</v>
+        <v>586.684667867193</v>
       </c>
       <c r="D14" t="n">
-        <v>189799.938542649</v>
+        <v>589.544480271554</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>-94897.1590708918</v>
+        <v>-292.342333933596</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -811,437 +811,89 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="n">
-        <v>82352.0425680329</v>
+        <v>389.800961060703</v>
       </c>
       <c r="D15" t="n">
-        <v>82366.5241714958</v>
+        <v>395.520585869427</v>
       </c>
       <c r="E15" t="n">
-        <v>-107444.275573751</v>
+        <v>-196.883706806489</v>
       </c>
       <c r="F15" t="n">
-        <v>-107433.414371154</v>
+        <v>-194.023894402128</v>
       </c>
       <c r="G15" t="n">
-        <v>-41172.0212840165</v>
+        <v>-192.900480530352</v>
       </c>
       <c r="H15" t="n">
-        <v>107444.275573751</v>
+        <v>196.883706806489</v>
       </c>
       <c r="I15" t="n">
-        <v>107433.414371154</v>
+        <v>194.023894402128</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n">
-        <v>6337.35754896603</v>
+        <v>425.961781358968</v>
       </c>
       <c r="D16" t="n">
-        <v>6385.31294534625</v>
+        <v>437.338529704802</v>
       </c>
       <c r="E16" t="n">
-        <v>-183458.960592818</v>
+        <v>-160.722886508225</v>
       </c>
       <c r="F16" t="n">
-        <v>-183414.625597303</v>
+        <v>-152.205950566753</v>
       </c>
       <c r="G16" t="n">
-        <v>-3152.67877448301</v>
+        <v>-208.980890679484</v>
       </c>
       <c r="H16" t="n">
-        <v>183458.960592818</v>
+        <v>160.722886508225</v>
       </c>
       <c r="I16" t="n">
-        <v>183414.625597303</v>
+        <v>152.205950566753</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C17" t="n">
-        <v>6157.4927272959</v>
+        <v>425.961781358968</v>
       </c>
       <c r="D17" t="n">
-        <v>6247.09355027078</v>
+        <v>437.338529704802</v>
       </c>
       <c r="E17" t="n">
-        <v>-183638.825414488</v>
+        <v>-160.722886508225</v>
       </c>
       <c r="F17" t="n">
-        <v>-183552.844992379</v>
+        <v>-152.205950566753</v>
       </c>
       <c r="G17" t="n">
-        <v>-3047.74636364795</v>
+        <v>-208.980890679484</v>
       </c>
       <c r="H17" t="n">
-        <v>183638.825414488</v>
+        <v>160.722886508225</v>
       </c>
       <c r="I17" t="n">
-        <v>183552.844992379</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="n">
-        <v>119396.850936627</v>
-      </c>
-      <c r="D18" t="n">
-        <v>119398.722137638</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-59697.4254683136</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="n">
-        <v>115863.294437099</v>
-      </c>
-      <c r="D19" t="n">
-        <v>115870.779241143</v>
-      </c>
-      <c r="E19" t="n">
-        <v>-3533.55649952796</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-3527.94289649522</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-57927.6472185496</v>
-      </c>
-      <c r="H19" t="n">
-        <v>3533.55649952796</v>
-      </c>
-      <c r="I19" t="n">
-        <v>3527.94289649522</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="n">
-        <v>109150.955636152</v>
-      </c>
-      <c r="D20" t="n">
-        <v>109150.341930513</v>
-      </c>
-      <c r="E20" t="n">
-        <v>-10245.8953004748</v>
-      </c>
-      <c r="F20" t="n">
-        <v>-10248.3802071246</v>
-      </c>
-      <c r="G20" t="n">
-        <v>-54574.4778180761</v>
-      </c>
-      <c r="H20" t="n">
-        <v>10245.8953004748</v>
-      </c>
-      <c r="I20" t="n">
-        <v>10248.3802071246</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="n">
-        <v>109150.955636152</v>
-      </c>
-      <c r="D21" t="n">
-        <v>109150.341930513</v>
-      </c>
-      <c r="E21" t="n">
-        <v>-10245.8953004748</v>
-      </c>
-      <c r="F21" t="n">
-        <v>-10248.3802071246</v>
-      </c>
-      <c r="G21" t="n">
-        <v>-54574.4778180761</v>
-      </c>
-      <c r="H21" t="n">
-        <v>10245.8953004748</v>
-      </c>
-      <c r="I21" t="n">
-        <v>10248.3802071246</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="n">
-        <v>9817492.65391331</v>
-      </c>
-      <c r="D22" t="n">
-        <v>9817496.17537423</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>-4908745.32695665</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="n">
-        <v>242380.234257061</v>
-      </c>
-      <c r="D23" t="n">
-        <v>242394.320100732</v>
-      </c>
-      <c r="E23" t="n">
-        <v>-9575112.41965625</v>
-      </c>
-      <c r="F23" t="n">
-        <v>-9575101.85527349</v>
-      </c>
-      <c r="G23" t="n">
-        <v>-121186.11712853</v>
-      </c>
-      <c r="H23" t="n">
-        <v>9575112.41965625</v>
-      </c>
-      <c r="I23" t="n">
-        <v>9575101.85527349</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" t="n">
-        <v>235109.006440944</v>
-      </c>
-      <c r="D24" t="n">
-        <v>235125.350851087</v>
-      </c>
-      <c r="E24" t="n">
-        <v>-9582383.64747236</v>
-      </c>
-      <c r="F24" t="n">
-        <v>-9582370.82452314</v>
-      </c>
-      <c r="G24" t="n">
-        <v>-117546.503220472</v>
-      </c>
-      <c r="H24" t="n">
-        <v>9582383.64747236</v>
-      </c>
-      <c r="I24" t="n">
-        <v>9582370.82452314</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="n">
-        <v>235109.006440944</v>
-      </c>
-      <c r="D25" t="n">
-        <v>235125.350851087</v>
-      </c>
-      <c r="E25" t="n">
-        <v>-9582383.64747236</v>
-      </c>
-      <c r="F25" t="n">
-        <v>-9582370.82452314</v>
-      </c>
-      <c r="G25" t="n">
-        <v>-117546.503220472</v>
-      </c>
-      <c r="H25" t="n">
-        <v>9582383.64747236</v>
-      </c>
-      <c r="I25" t="n">
-        <v>9582370.82452314</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1328.1060261503</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1330.96583855466</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>-663.05301307515</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1131.26013147114</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1136.97975627986</v>
-      </c>
-      <c r="E27" t="n">
-        <v>-196.84589467916</v>
-      </c>
-      <c r="F27" t="n">
-        <v>-193.986082274798</v>
-      </c>
-      <c r="G27" t="n">
-        <v>-563.63006573557</v>
-      </c>
-      <c r="H27" t="n">
-        <v>196.84589467916</v>
-      </c>
-      <c r="I27" t="n">
-        <v>193.986082274798</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1154.91358263294</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1166.29033097877</v>
-      </c>
-      <c r="E28" t="n">
-        <v>-173.192443517362</v>
-      </c>
-      <c r="F28" t="n">
-        <v>-164.675507575889</v>
-      </c>
-      <c r="G28" t="n">
-        <v>-573.456791316469</v>
-      </c>
-      <c r="H28" t="n">
-        <v>173.192443517362</v>
-      </c>
-      <c r="I28" t="n">
-        <v>164.675507575889</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1154.91358263294</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1166.29033097877</v>
-      </c>
-      <c r="E29" t="n">
-        <v>-173.192443517362</v>
-      </c>
-      <c r="F29" t="n">
-        <v>-164.675507575889</v>
-      </c>
-      <c r="G29" t="n">
-        <v>-573.456791316469</v>
-      </c>
-      <c r="H29" t="n">
-        <v>173.192443517362</v>
-      </c>
-      <c r="I29" t="n">
-        <v>164.675507575889</v>
+        <v>152.205950566753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>